<commit_message>
109 features so far
</commit_message>
<xml_diff>
--- a/trainingdata.xlsx
+++ b/trainingdata.xlsx
@@ -336,15 +336,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X517"/>
+  <dimension ref="A1:DD517"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A505" workbookViewId="0">
-      <selection activeCell="A517" sqref="A517:X517"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:DD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:108" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>74</v>
       </c>
@@ -352,73 +352,325 @@
         <v>0</v>
       </c>
       <c r="C1">
-        <v>155.91859362730114</v>
+        <v>155.46848424159677</v>
       </c>
       <c r="D1">
-        <v>174.6501919807155</v>
+        <v>173.0369937383195</v>
       </c>
       <c r="E1">
-        <v>-136.93163716301123</v>
+        <v>-137.65809292648964</v>
       </c>
       <c r="F1">
-        <v>-145.80698262388105</v>
+        <v>-140.69908770149817</v>
       </c>
       <c r="G1">
-        <v>37.406355705772768</v>
+        <v>37.442452615428699</v>
       </c>
       <c r="H1">
-        <v>36.773604729433757</v>
+        <v>37.710487317468157</v>
       </c>
       <c r="I1">
-        <v>-6.2685251644293043</v>
+        <v>-41.236795671296242</v>
       </c>
       <c r="J1">
-        <v>51.228056801020571</v>
+        <v>-102.75373495352937</v>
       </c>
       <c r="K1">
-        <v>135.21170442470839</v>
+        <v>135.78444192024108</v>
       </c>
       <c r="L1">
-        <v>117.48947474793893</v>
+        <v>118.75213160097718</v>
       </c>
       <c r="M1">
-        <v>68.416905423224478</v>
+        <v>68.418024967644357</v>
       </c>
       <c r="N1">
-        <v>67.323354541777334</v>
+        <v>68.061209885220961</v>
       </c>
       <c r="O1">
-        <v>165.996952363839</v>
+        <v>172.08967983996681</v>
       </c>
       <c r="P1">
-        <v>99.425747131872669</v>
+        <v>164.71867419050903</v>
       </c>
       <c r="Q1">
-        <v>636285.22429145628</v>
+        <v>642235.20854000968</v>
       </c>
       <c r="R1">
-        <v>33949823.468918286</v>
+        <v>37845429.422799274</v>
       </c>
       <c r="S1">
-        <v>529515.44927893463</v>
+        <v>488110.63730681612</v>
       </c>
       <c r="T1">
-        <v>38308071.174504384</v>
+        <v>34553161.683952093</v>
       </c>
       <c r="U1">
-        <v>264663.63743326801</v>
+        <v>283458.10063371988</v>
       </c>
       <c r="V1">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="W1">
-        <v>132059663.84147742</v>
+        <v>126419751.39391948</v>
       </c>
       <c r="X1">
-        <v>5506784.4233586602</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+        <v>5488921.5859200405</v>
+      </c>
+      <c r="Y1">
+        <v>293.83999999999997</v>
+      </c>
+      <c r="Z1">
+        <v>294.69346786109799</v>
+      </c>
+      <c r="AA1">
+        <v>23</v>
+      </c>
+      <c r="AB1">
+        <v>92</v>
+      </c>
+      <c r="AC1">
+        <v>4.160000000000025</v>
+      </c>
+      <c r="AD1">
+        <v>1.4007916826739686</v>
+      </c>
+      <c r="AE1">
+        <v>293.83999999999997</v>
+      </c>
+      <c r="AF1">
+        <v>298.375</v>
+      </c>
+      <c r="AG1">
+        <v>298.38684343203425</v>
+      </c>
+      <c r="AH1">
+        <v>23</v>
+      </c>
+      <c r="AI1">
+        <v>95.833333333333343</v>
+      </c>
+      <c r="AJ1">
+        <v>0.375</v>
+      </c>
+      <c r="AK1">
+        <v>0.24621291455268557</v>
+      </c>
+      <c r="AL1">
+        <v>298.375</v>
+      </c>
+      <c r="AM1">
+        <v>298.375</v>
+      </c>
+      <c r="AN1">
+        <v>298.65511045351292</v>
+      </c>
+      <c r="AO1">
+        <v>22</v>
+      </c>
+      <c r="AP1">
+        <v>91.666666666666657</v>
+      </c>
+      <c r="AQ1">
+        <v>1.625</v>
+      </c>
+      <c r="AR1">
+        <v>0.91003541047679515</v>
+      </c>
+      <c r="AS1">
+        <v>298.375</v>
+      </c>
+      <c r="AT1">
+        <v>296</v>
+      </c>
+      <c r="AU1">
+        <v>296.24962447233582</v>
+      </c>
+      <c r="AV1">
+        <v>23</v>
+      </c>
+      <c r="AW1">
+        <v>92</v>
+      </c>
+      <c r="AX1">
+        <v>3</v>
+      </c>
+      <c r="AY1">
+        <v>0.94109741978607431</v>
+      </c>
+      <c r="AZ1">
+        <v>296</v>
+      </c>
+      <c r="BA1">
+        <v>293.92</v>
+      </c>
+      <c r="BB1">
+        <v>294.72753519140355</v>
+      </c>
+      <c r="BC1">
+        <v>23</v>
+      </c>
+      <c r="BD1">
+        <v>92</v>
+      </c>
+      <c r="BE1">
+        <v>4.0799999999999841</v>
+      </c>
+      <c r="BF1">
+        <v>1.3778848681347777</v>
+      </c>
+      <c r="BG1">
+        <v>293.92</v>
+      </c>
+      <c r="BH1">
+        <v>298.41666666666669</v>
+      </c>
+      <c r="BI1">
+        <v>298.64094941361719</v>
+      </c>
+      <c r="BJ1">
+        <v>23</v>
+      </c>
+      <c r="BK1">
+        <v>95.833333333333343</v>
+      </c>
+      <c r="BL1">
+        <v>0.58333333333331439</v>
+      </c>
+      <c r="BM1">
+        <v>0.86254635125135726</v>
+      </c>
+      <c r="BN1">
+        <v>298.41666666666669</v>
+      </c>
+      <c r="BO1">
+        <v>296.92</v>
+      </c>
+      <c r="BP1">
+        <v>297.01521846531699</v>
+      </c>
+      <c r="BQ1">
+        <v>24</v>
+      </c>
+      <c r="BR1">
+        <v>96</v>
+      </c>
+      <c r="BS1">
+        <v>2.0799999999999841</v>
+      </c>
+      <c r="BT1">
+        <v>0.6516305193691827</v>
+      </c>
+      <c r="BU1">
+        <v>296.92</v>
+      </c>
+      <c r="BV1">
+        <v>295.60000000000002</v>
+      </c>
+      <c r="BW1">
+        <v>295.9259366801092</v>
+      </c>
+      <c r="BX1">
+        <v>23</v>
+      </c>
+      <c r="BY1">
+        <v>92</v>
+      </c>
+      <c r="BZ1">
+        <v>3.3999999999999773</v>
+      </c>
+      <c r="CA1">
+        <v>1.0320026018007256</v>
+      </c>
+      <c r="CB1">
+        <v>295.60000000000002</v>
+      </c>
+      <c r="CC1">
+        <v>298.375</v>
+      </c>
+      <c r="CD1">
+        <v>298.38879838224489</v>
+      </c>
+      <c r="CE1">
+        <v>23</v>
+      </c>
+      <c r="CF1">
+        <v>95.833333333333343</v>
+      </c>
+      <c r="CG1">
+        <v>0.625</v>
+      </c>
+      <c r="CH1">
+        <v>0.25867534773690271</v>
+      </c>
+      <c r="CI1">
+        <v>298.375</v>
+      </c>
+      <c r="CJ1">
+        <v>293.76</v>
+      </c>
+      <c r="CK1">
+        <v>294.64120553649656</v>
+      </c>
+      <c r="CL1">
+        <v>23</v>
+      </c>
+      <c r="CM1">
+        <v>92</v>
+      </c>
+      <c r="CN1">
+        <v>5.2400000000000091</v>
+      </c>
+      <c r="CO1">
+        <v>1.4139433276402305</v>
+      </c>
+      <c r="CP1">
+        <v>293.76</v>
+      </c>
+      <c r="CQ1">
+        <v>293.72000000000003</v>
+      </c>
+      <c r="CR1">
+        <v>294.61602128872761</v>
+      </c>
+      <c r="CS1">
+        <v>23</v>
+      </c>
+      <c r="CT1">
+        <v>92</v>
+      </c>
+      <c r="CU1">
+        <v>4.2799999999999727</v>
+      </c>
+      <c r="CV1">
+        <v>1.42084470206262</v>
+      </c>
+      <c r="CW1">
+        <v>293.72000000000003</v>
+      </c>
+      <c r="CX1">
+        <v>298.375</v>
+      </c>
+      <c r="CY1">
+        <v>298.3869830717598</v>
+      </c>
+      <c r="CZ1">
+        <v>23</v>
+      </c>
+      <c r="DA1">
+        <v>95.833333333333343</v>
+      </c>
+      <c r="DB1">
+        <v>0.375</v>
+      </c>
+      <c r="DC1">
+        <v>0.24286293168589015</v>
+      </c>
+      <c r="DD1">
+        <v>298.375</v>
+      </c>
+    </row>
+    <row r="2" spans="1:108" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>49</v>
       </c>
@@ -492,7 +744,7 @@
         <v>10329878.068327796</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:108" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>81</v>
       </c>
@@ -566,7 +818,7 @@
         <v>5990694.8792918259</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:108" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>45</v>
       </c>
@@ -640,7 +892,7 @@
         <v>15276189.185099922</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:108" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>53</v>
       </c>
@@ -714,7 +966,7 @@
         <v>13951734.017597683</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:108" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>29</v>
       </c>
@@ -788,7 +1040,7 @@
         <v>29716548.496092722</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:108" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>74</v>
       </c>
@@ -862,7 +1114,7 @@
         <v>9156094.9184415638</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:108" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>80</v>
       </c>
@@ -936,7 +1188,7 @@
         <v>23761783.930400953</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:108" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>81</v>
       </c>
@@ -1010,7 +1262,7 @@
         <v>25337394.075597178</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:108" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>82</v>
       </c>
@@ -1084,7 +1336,7 @@
         <v>21409608.771072324</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:108" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>87</v>
       </c>
@@ -1158,7 +1410,7 @@
         <v>26708501.591055259</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:108" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>74</v>
       </c>
@@ -1232,7 +1484,7 @@
         <v>14721242.267327577</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:108" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>57</v>
       </c>
@@ -1306,7 +1558,7 @@
         <v>16096808.491076363</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:108" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>76</v>
       </c>
@@ -1380,7 +1632,7 @@
         <v>16307155.281153316</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:108" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>41</v>
       </c>
@@ -1454,7 +1706,7 @@
         <v>14999142.029852752</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:108" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>

</xml_diff>